<commit_message>
two animals didn't have absolute mono numbers even though they had cbcs, so i just calculated it in the sheet. I mean, that htey had %mono and total WBC in the sheet, but somehow the calculation was not already reported
</commit_message>
<xml_diff>
--- a/data/raw/cbc_csf1r.xlsx
+++ b/data/raw/cbc_csf1r.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewding/Desktop/Projects/2024 BrdU lifetime/2024-07-11 AIDS symposium abstract/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A5C2555-B170-C24C-B37D-7299CDFE2D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD629F3F-CF6E-3341-AE28-EEFA81BE002E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="14720" xr2:uid="{1CBF3651-0C16-D64A-9808-75225D46922A}"/>
+    <workbookView xWindow="1580" yWindow="920" windowWidth="26840" windowHeight="14720" xr2:uid="{1CBF3651-0C16-D64A-9808-75225D46922A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4518,8 +4518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA08941F-5D74-7E41-99CA-FB214A663AE3}">
   <dimension ref="A1:AX204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AX1048576"/>
+    <sheetView tabSelected="1" topLeftCell="M179" workbookViewId="0">
+      <selection activeCell="X196" sqref="X196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21528,7 +21528,10 @@
       <c r="Y201" s="7"/>
       <c r="Z201" s="7"/>
       <c r="AA201" s="7"/>
-      <c r="AB201" s="7"/>
+      <c r="AB201" s="7">
+        <f>T201/100*F201</f>
+        <v>0.24239999999999998</v>
+      </c>
       <c r="AC201" s="7"/>
       <c r="AD201" s="7"/>
       <c r="AE201" s="7"/>
@@ -21734,7 +21737,10 @@
       <c r="Y203" s="7"/>
       <c r="Z203" s="7"/>
       <c r="AA203" s="7"/>
-      <c r="AB203" s="7"/>
+      <c r="AB203" s="7">
+        <f>T203/100*F203</f>
+        <v>0.40949999999999998</v>
+      </c>
       <c r="AC203" s="7"/>
       <c r="AD203" s="7"/>
       <c r="AE203" s="7"/>

</xml_diff>